<commit_message>
added jer's comments 26092013
</commit_message>
<xml_diff>
--- a/ansonia/Table 1.xlsx
+++ b/ansonia/Table 1.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1716" yWindow="444" windowWidth="23256" windowHeight="13176" tabRatio="500"/>
+    <workbookView xWindow="1720" yWindow="440" windowWidth="23260" windowHeight="13180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>Primer name</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>16S1M</t>
-  </si>
-  <si>
-    <t>(Fu, 2000)</t>
   </si>
   <si>
     <t>AAARCATKGGTCTTGTAARCC</t>
@@ -137,14 +134,14 @@
     <t>Primer reference</t>
   </si>
   <si>
-    <t>Table 1.  Primers used in this study for PCR amplification and sequencing reactions.</t>
+    <t>(Fu 2000)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -194,23 +191,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -238,15 +224,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -590,88 +573,94 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.69921875" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
@@ -680,12 +669,12 @@
         <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
@@ -699,7 +688,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>6</v>
@@ -708,44 +697,27 @@
         <v>19</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="C14" s="1"/>
+      <c r="D9" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="C13" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>